<commit_message>
Desc stats and boxplots are fixed
</commit_message>
<xml_diff>
--- a/1. R/1. EDA/desc_stats.xlsx
+++ b/1. R/1. EDA/desc_stats.xlsx
@@ -3,23 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\RProjects\Diploma_Holland\1. R\1. EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="upd" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="4" r:id="rId1"/>
+    <sheet name="Old" sheetId="1" r:id="rId2"/>
+    <sheet name="All" r:id="rId6" sheetId="5"/>
+    <sheet name="Шварц" r:id="rId7" sheetId="6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="408">
   <si>
     <t>#</t>
   </si>
@@ -742,12 +745,514 @@
   </si>
   <si>
     <t>0,24</t>
+  </si>
+  <si>
+    <t>Mean (SD)</t>
+  </si>
+  <si>
+    <t>Median (IQR)</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>16-факторный опросник Кеттелла</t>
+  </si>
+  <si>
+    <t>Пятифакторный опросник личности</t>
+  </si>
+  <si>
+    <t>Гипертимность</t>
+  </si>
+  <si>
+    <t>Дистимность</t>
+  </si>
+  <si>
+    <t>Циклотимность</t>
+  </si>
+  <si>
+    <t>Неуравновешенность</t>
+  </si>
+  <si>
+    <t>Застревание</t>
+  </si>
+  <si>
+    <t>Эмотивность</t>
+  </si>
+  <si>
+    <t>Экзальтированность</t>
+  </si>
+  <si>
+    <t>Тревожность</t>
+  </si>
+  <si>
+    <t>Педантичность</t>
+  </si>
+  <si>
+    <t>Демонстративность</t>
+  </si>
+  <si>
+    <t>6,61 (2,41)</t>
+  </si>
+  <si>
+    <t>7,26 (2,21)</t>
+  </si>
+  <si>
+    <t>6,89 (2,14)</t>
+  </si>
+  <si>
+    <t>6,88 (1,99)</t>
+  </si>
+  <si>
+    <t>6,88 (2,35)</t>
+  </si>
+  <si>
+    <t>7,48 (2,82)</t>
+  </si>
+  <si>
+    <t>12,79 (6,55)</t>
+  </si>
+  <si>
+    <t>14,6 (4,3)</t>
+  </si>
+  <si>
+    <t>14,35 (5,35)</t>
+  </si>
+  <si>
+    <t>12,46 (4,94)</t>
+  </si>
+  <si>
+    <t>11,35 (6,14)</t>
+  </si>
+  <si>
+    <t>14,41 (5,97)</t>
+  </si>
+  <si>
+    <t>13,85 (4,65)</t>
+  </si>
+  <si>
+    <t>13,53 (5,55)</t>
+  </si>
+  <si>
+    <t>12,88 (4,66)</t>
+  </si>
+  <si>
+    <t>14,76 (6,16)</t>
+  </si>
+  <si>
+    <t>11,3 (5,62)</t>
+  </si>
+  <si>
+    <t>6,48 (3,41)</t>
+  </si>
+  <si>
+    <t>16,14 (6,13)</t>
+  </si>
+  <si>
+    <t>10,91 (4,17)</t>
+  </si>
+  <si>
+    <t>9,87 (3,71)</t>
+  </si>
+  <si>
+    <t>13,44 (4,91)</t>
+  </si>
+  <si>
+    <t>12,88 (4,02)</t>
+  </si>
+  <si>
+    <t>12,51 (4,32)</t>
+  </si>
+  <si>
+    <t>10,55 (3,55)</t>
+  </si>
+  <si>
+    <t>11,15 (6,19)</t>
+  </si>
+  <si>
+    <t>11,98 (3,6)</t>
+  </si>
+  <si>
+    <t>10,59 (3,39)</t>
+  </si>
+  <si>
+    <t>10,76 (3,02)</t>
+  </si>
+  <si>
+    <t>10,18 (2,97)</t>
+  </si>
+  <si>
+    <t>13,68 (5,39)</t>
+  </si>
+  <si>
+    <t>10,43 (2,77)</t>
+  </si>
+  <si>
+    <t>12,43 (3,75)</t>
+  </si>
+  <si>
+    <t>11,29 (3,53)</t>
+  </si>
+  <si>
+    <t>13,94 (5,55)</t>
+  </si>
+  <si>
+    <t>7,68 (2,3)</t>
+  </si>
+  <si>
+    <t>42,76 (11,96)</t>
+  </si>
+  <si>
+    <t>49,8 (11,84)</t>
+  </si>
+  <si>
+    <t>51,53 (11,64)</t>
+  </si>
+  <si>
+    <t>51,49 (15,01)</t>
+  </si>
+  <si>
+    <t>54,42 (8,89)</t>
+  </si>
+  <si>
+    <t>38,78 (9,85)</t>
+  </si>
+  <si>
+    <t>25,5 (5,94)</t>
+  </si>
+  <si>
+    <t>15,63 (6,6)</t>
+  </si>
+  <si>
+    <t>14,65 (4,83)</t>
+  </si>
+  <si>
+    <t>26,59 (5,33)</t>
+  </si>
+  <si>
+    <t>11,46 (5,08)</t>
+  </si>
+  <si>
+    <t>17,56 (5,81)</t>
+  </si>
+  <si>
+    <t>17,78 (8,36)</t>
+  </si>
+  <si>
+    <t>24,45 (7,17)</t>
+  </si>
+  <si>
+    <t>19,32 (5,64)</t>
+  </si>
+  <si>
+    <t>11,15 (3,34)</t>
+  </si>
+  <si>
+    <t>4,5 (3,87)</t>
+  </si>
+  <si>
+    <t>13,85 (5,76)</t>
+  </si>
+  <si>
+    <t>8,5 (4,59)</t>
+  </si>
+  <si>
+    <t>11,09 (4,98)</t>
+  </si>
+  <si>
+    <t>5,37 (3,55)</t>
+  </si>
+  <si>
+    <t>6,52 (4,4)</t>
+  </si>
+  <si>
+    <t>4,84 (4,59)</t>
+  </si>
+  <si>
+    <t>7,53 (3,28)</t>
+  </si>
+  <si>
+    <t>8,42 (4,24)</t>
+  </si>
+  <si>
+    <t>7 (5-8)</t>
+  </si>
+  <si>
+    <t>7 (6-9)</t>
+  </si>
+  <si>
+    <t>7 (5-9)</t>
+  </si>
+  <si>
+    <t>8 (5,5-10)</t>
+  </si>
+  <si>
+    <t>15 (9-18)</t>
+  </si>
+  <si>
+    <t>14 (12-18)</t>
+  </si>
+  <si>
+    <t>15 (12-18)</t>
+  </si>
+  <si>
+    <t>12 (8-16)</t>
+  </si>
+  <si>
+    <t>12 (6-15)</t>
+  </si>
+  <si>
+    <t>14 (10-18)</t>
+  </si>
+  <si>
+    <t>12 (9-15)</t>
+  </si>
+  <si>
+    <t>12 (12-18)</t>
+  </si>
+  <si>
+    <t>11 (7-16)</t>
+  </si>
+  <si>
+    <t>6 (4-8)</t>
+  </si>
+  <si>
+    <t>17 (12-21)</t>
+  </si>
+  <si>
+    <t>11 (8-13,5)</t>
+  </si>
+  <si>
+    <t>10 (7-12)</t>
+  </si>
+  <si>
+    <t>13 (10-17)</t>
+  </si>
+  <si>
+    <t>13 (10-16)</t>
+  </si>
+  <si>
+    <t>12 (10-16)</t>
+  </si>
+  <si>
+    <t>11 (8-13)</t>
+  </si>
+  <si>
+    <t>11 (6-15,5)</t>
+  </si>
+  <si>
+    <t>12 (10-15)</t>
+  </si>
+  <si>
+    <t>10 (8-13)</t>
+  </si>
+  <si>
+    <t>11 (9-13)</t>
+  </si>
+  <si>
+    <t>10 (8-12)</t>
+  </si>
+  <si>
+    <t>10 (9-12)</t>
+  </si>
+  <si>
+    <t>13 (10-15)</t>
+  </si>
+  <si>
+    <t>11 (9-14)</t>
+  </si>
+  <si>
+    <t>8 (6-9)</t>
+  </si>
+  <si>
+    <t>42 (34-51)</t>
+  </si>
+  <si>
+    <t>50 (42-58)</t>
+  </si>
+  <si>
+    <t>51 (43-61)</t>
+  </si>
+  <si>
+    <t>53 (41,5-63,5)</t>
+  </si>
+  <si>
+    <t>54 (49-61)</t>
+  </si>
+  <si>
+    <t>39 (33-46)</t>
+  </si>
+  <si>
+    <t>26 (23-29,5)</t>
+  </si>
+  <si>
+    <t>16 (11-20,5)</t>
+  </si>
+  <si>
+    <t>16 (12-18)</t>
+  </si>
+  <si>
+    <t>27 (23,5-30)</t>
+  </si>
+  <si>
+    <t>12 (8-15)</t>
+  </si>
+  <si>
+    <t>18 (14-22)</t>
+  </si>
+  <si>
+    <t>18 (12-23)</t>
+  </si>
+  <si>
+    <t>25 (21-30)</t>
+  </si>
+  <si>
+    <t>20 (16-23)</t>
+  </si>
+  <si>
+    <t>12 (9-14)</t>
+  </si>
+  <si>
+    <t>4 (1,5-7)</t>
+  </si>
+  <si>
+    <t>14 (9,5-18)</t>
+  </si>
+  <si>
+    <t>9 (5-12)</t>
+  </si>
+  <si>
+    <t>11 (7,5-15)</t>
+  </si>
+  <si>
+    <t>5 (3-8)</t>
+  </si>
+  <si>
+    <t>6 (3-10)</t>
+  </si>
+  <si>
+    <t>4 (1-8)</t>
+  </si>
+  <si>
+    <t>8 (5-10)</t>
+  </si>
+  <si>
+    <t>Безопасность</t>
+  </si>
+  <si>
+    <t>Власть</t>
+  </si>
+  <si>
+    <t>Гедонизм</t>
+  </si>
+  <si>
+    <t>Доброта</t>
+  </si>
+  <si>
+    <t>Достижение</t>
+  </si>
+  <si>
+    <t>Конформность</t>
+  </si>
+  <si>
+    <t>Самостоятельность</t>
+  </si>
+  <si>
+    <t>Стимуляция</t>
+  </si>
+  <si>
+    <t>Традиция</t>
+  </si>
+  <si>
+    <t>Универсализм</t>
+  </si>
+  <si>
+    <t>индивидуальный приоритет</t>
+  </si>
+  <si>
+    <t>нормативный идеал</t>
+  </si>
+  <si>
+    <t>Эмоциональная устойчивость - эмоциональная неустойчивость</t>
+  </si>
+  <si>
+    <t>Реалистический (R)</t>
+  </si>
+  <si>
+    <t>Исследовательский (I)</t>
+  </si>
+  <si>
+    <t>Артистический (A)</t>
+  </si>
+  <si>
+    <t>Социальный (S)</t>
+  </si>
+  <si>
+    <t>Предприимчивый (E)</t>
+  </si>
+  <si>
+    <t>Традиционный (C)</t>
+  </si>
+  <si>
+    <t>Открытость - Замкнутость</t>
+  </si>
+  <si>
+    <t>Эмоциональная стабильность - Эмоциональная неустойчивость</t>
+  </si>
+  <si>
+    <t>Независимость - Податливость</t>
+  </si>
+  <si>
+    <t>Беспечность - Озабоченность</t>
+  </si>
+  <si>
+    <t>Сознательность - Беспринципность</t>
+  </si>
+  <si>
+    <t>Смелость - Застенчивость</t>
+  </si>
+  <si>
+    <t>Чувственность - Твердость</t>
+  </si>
+  <si>
+    <t>Подозрительность - Доверчивость</t>
+  </si>
+  <si>
+    <t>Мечтательность - Практичность</t>
+  </si>
+  <si>
+    <t>Утонченность - Простота</t>
+  </si>
+  <si>
+    <t>Склонность к чувству вины - Спокойная самоуверенность</t>
+  </si>
+  <si>
+    <t>Радикализм - Консерватизм</t>
+  </si>
+  <si>
+    <t>Самостоятельность - Зависимость от группы</t>
+  </si>
+  <si>
+    <t>Самоконтроль, сильная воля - Недостаток самоконтроля, индифферентность</t>
+  </si>
+  <si>
+    <t>Внутренняя напряженность - Внутренняя расслабленность</t>
+  </si>
+  <si>
+    <t>Развитое мышление - Ограниченное мышление</t>
+  </si>
+  <si>
+    <t>norm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -816,9 +1321,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -827,6 +1329,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1108,51 +1613,1329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="32" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.6640625" collapsed="true"/>
+    <col min="8" max="10" customWidth="true" width="18.88671875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>244</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M1" t="s">
+        <v>243</v>
+      </c>
+      <c r="N1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" t="s">
+        <v>263</v>
+      </c>
+      <c r="L2" t="s">
+        <v>322</v>
+      </c>
+      <c r="M2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" t="s">
+        <v>248</v>
+      </c>
+      <c r="K3" t="s">
+        <v>264</v>
+      </c>
+      <c r="L3" t="s">
+        <v>323</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" t="s">
+        <v>249</v>
+      </c>
+      <c r="K4" t="s">
+        <v>265</v>
+      </c>
+      <c r="L4" t="s">
+        <v>324</v>
+      </c>
+      <c r="M4" t="s">
+        <v>135</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" t="s">
+        <v>250</v>
+      </c>
+      <c r="K5" t="s">
+        <v>266</v>
+      </c>
+      <c r="L5" t="s">
+        <v>325</v>
+      </c>
+      <c r="M5" t="s">
+        <v>135</v>
+      </c>
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s">
+        <v>251</v>
+      </c>
+      <c r="K6" t="s">
+        <v>267</v>
+      </c>
+      <c r="L6" t="s">
+        <v>326</v>
+      </c>
+      <c r="M6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" t="s">
+        <v>321</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K7" t="s">
+        <v>268</v>
+      </c>
+      <c r="L7" t="s">
+        <v>322</v>
+      </c>
+      <c r="M7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" t="s">
+        <v>253</v>
+      </c>
+      <c r="K8" t="s">
+        <v>269</v>
+      </c>
+      <c r="L8" t="s">
+        <v>327</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D9" t="s">
+        <v>349</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H9" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" t="s">
+        <v>254</v>
+      </c>
+      <c r="K9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L9" t="s">
+        <v>322</v>
+      </c>
+      <c r="M9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" t="s">
+        <v>350</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>255</v>
+      </c>
+      <c r="K10" t="s">
+        <v>271</v>
+      </c>
+      <c r="L10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M10" t="s">
+        <v>135</v>
+      </c>
+      <c r="N10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" t="s">
+        <v>296</v>
+      </c>
+      <c r="D11" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>256</v>
+      </c>
+      <c r="K11" t="s">
+        <v>272</v>
+      </c>
+      <c r="L11" t="s">
+        <v>329</v>
+      </c>
+      <c r="M11" t="s">
+        <v>135</v>
+      </c>
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I12" t="s">
+        <v>372</v>
+      </c>
+      <c r="J12" t="s">
+        <v>382</v>
+      </c>
+      <c r="K12" t="s">
+        <v>312</v>
+      </c>
+      <c r="L12" t="s">
+        <v>367</v>
+      </c>
+      <c r="M12" t="s">
+        <v>136</v>
+      </c>
+      <c r="N12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>373</v>
+      </c>
+      <c r="J13" t="s">
+        <v>382</v>
+      </c>
+      <c r="K13" t="s">
+        <v>309</v>
+      </c>
+      <c r="L13" t="s">
+        <v>364</v>
+      </c>
+      <c r="M13" t="s">
+        <v>138</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>274</v>
+      </c>
+      <c r="D14" t="s">
+        <v>331</v>
+      </c>
+      <c r="E14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" t="s">
+        <v>374</v>
+      </c>
+      <c r="J14" t="s">
+        <v>382</v>
+      </c>
+      <c r="K14" t="s">
+        <v>316</v>
+      </c>
+      <c r="L14" t="s">
+        <v>371</v>
+      </c>
+      <c r="M14" t="s">
+        <v>138</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>275</v>
+      </c>
+      <c r="D15" t="s">
+        <v>332</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>375</v>
+      </c>
+      <c r="J15" t="s">
+        <v>382</v>
+      </c>
+      <c r="K15" t="s">
+        <v>317</v>
+      </c>
+      <c r="L15" t="s">
+        <v>366</v>
+      </c>
+      <c r="M15" t="s">
+        <v>140</v>
+      </c>
+      <c r="N15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" t="s">
+        <v>276</v>
+      </c>
+      <c r="D16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" t="s">
+        <v>376</v>
+      </c>
+      <c r="J16" t="s">
+        <v>382</v>
+      </c>
+      <c r="K16" t="s">
+        <v>311</v>
+      </c>
+      <c r="L16" t="s">
+        <v>366</v>
+      </c>
+      <c r="M16" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" t="s">
+        <v>334</v>
+      </c>
+      <c r="E17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" t="s">
+        <v>377</v>
+      </c>
+      <c r="J17" t="s">
+        <v>382</v>
+      </c>
+      <c r="K17" t="s">
+        <v>314</v>
+      </c>
+      <c r="L17" t="s">
+        <v>369</v>
+      </c>
+      <c r="M17" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D18" t="s">
+        <v>335</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>378</v>
+      </c>
+      <c r="J18" t="s">
+        <v>382</v>
+      </c>
+      <c r="K18" t="s">
+        <v>308</v>
+      </c>
+      <c r="L18" t="s">
+        <v>363</v>
+      </c>
+      <c r="M18" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" t="s">
+        <v>379</v>
+      </c>
+      <c r="J19" t="s">
+        <v>382</v>
+      </c>
+      <c r="K19" t="s">
+        <v>313</v>
+      </c>
+      <c r="L19" t="s">
+        <v>368</v>
+      </c>
+      <c r="M19" t="s">
+        <v>138</v>
+      </c>
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+      <c r="D20" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" t="s">
+        <v>380</v>
+      </c>
+      <c r="J20" t="s">
+        <v>382</v>
+      </c>
+      <c r="K20" t="s">
+        <v>315</v>
+      </c>
+      <c r="L20" t="s">
+        <v>370</v>
+      </c>
+      <c r="M20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>245</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>281</v>
+      </c>
+      <c r="D21" t="s">
+        <v>338</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" t="s">
+        <v>381</v>
+      </c>
+      <c r="J21" t="s">
+        <v>382</v>
+      </c>
+      <c r="K21" t="s">
+        <v>310</v>
+      </c>
+      <c r="L21" t="s">
+        <v>365</v>
+      </c>
+      <c r="M21" t="s">
+        <v>136</v>
+      </c>
+      <c r="N21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>282</v>
+      </c>
+      <c r="D22" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" t="s">
+        <v>372</v>
+      </c>
+      <c r="J22" t="s">
+        <v>383</v>
+      </c>
+      <c r="K22" t="s">
+        <v>299</v>
+      </c>
+      <c r="L22" t="s">
+        <v>354</v>
+      </c>
+      <c r="M22" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" t="s">
+        <v>283</v>
+      </c>
+      <c r="D23" t="s">
+        <v>340</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" t="s">
+        <v>373</v>
+      </c>
+      <c r="J23" t="s">
+        <v>383</v>
+      </c>
+      <c r="K23" t="s">
+        <v>300</v>
+      </c>
+      <c r="L23" t="s">
+        <v>355</v>
+      </c>
+      <c r="M23" t="s">
+        <v>136</v>
+      </c>
+      <c r="N23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>284</v>
+      </c>
+      <c r="D24" t="s">
+        <v>341</v>
+      </c>
+      <c r="E24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" t="s">
+        <v>374</v>
+      </c>
+      <c r="J24" t="s">
+        <v>383</v>
+      </c>
+      <c r="K24" t="s">
+        <v>301</v>
+      </c>
+      <c r="L24" t="s">
+        <v>356</v>
+      </c>
+      <c r="M24" t="s">
+        <v>137</v>
+      </c>
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" t="s">
+        <v>375</v>
+      </c>
+      <c r="J25" t="s">
+        <v>383</v>
+      </c>
+      <c r="K25" t="s">
+        <v>306</v>
+      </c>
+      <c r="L25" t="s">
+        <v>361</v>
+      </c>
+      <c r="M25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" t="s">
+        <v>343</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" t="s">
+        <v>376</v>
+      </c>
+      <c r="J26" t="s">
+        <v>383</v>
+      </c>
+      <c r="K26" t="s">
+        <v>307</v>
+      </c>
+      <c r="L26" t="s">
+        <v>362</v>
+      </c>
+      <c r="M26" t="s">
+        <v>138</v>
+      </c>
+      <c r="N26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>245</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D27" t="s">
+        <v>327</v>
+      </c>
+      <c r="E27" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" t="s">
+        <v>377</v>
+      </c>
+      <c r="J27" t="s">
+        <v>383</v>
+      </c>
+      <c r="K27" t="s">
+        <v>304</v>
+      </c>
+      <c r="L27" t="s">
+        <v>359</v>
+      </c>
+      <c r="M27" t="s">
+        <v>135</v>
+      </c>
+      <c r="N27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>288</v>
+      </c>
+      <c r="D28" t="s">
+        <v>344</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" t="s">
+        <v>378</v>
+      </c>
+      <c r="J28" t="s">
+        <v>383</v>
+      </c>
+      <c r="K28" t="s">
+        <v>302</v>
+      </c>
+      <c r="L28" t="s">
+        <v>357</v>
+      </c>
+      <c r="M28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D29" t="s">
+        <v>345</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" t="s">
+        <v>379</v>
+      </c>
+      <c r="J29" t="s">
+        <v>383</v>
+      </c>
+      <c r="K29" t="s">
+        <v>303</v>
+      </c>
+      <c r="L29" t="s">
+        <v>358</v>
+      </c>
+      <c r="M29" t="s">
+        <v>138</v>
+      </c>
+      <c r="N29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30" t="s">
+        <v>346</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I30" t="s">
+        <v>380</v>
+      </c>
+      <c r="J30" t="s">
+        <v>383</v>
+      </c>
+      <c r="K30" t="s">
+        <v>305</v>
+      </c>
+      <c r="L30" t="s">
+        <v>360</v>
+      </c>
+      <c r="M30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>245</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D31" t="s">
+        <v>327</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" t="s">
+        <v>381</v>
+      </c>
+      <c r="J31" t="s">
+        <v>383</v>
+      </c>
+      <c r="K31" t="s">
+        <v>298</v>
+      </c>
+      <c r="L31" t="s">
+        <v>353</v>
+      </c>
+      <c r="M31" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" t="s">
+        <v>347</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" style="1" width="8.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="38.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1160,7 +2943,7 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1195,7 +2978,7 @@
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="5" t="s">
         <v>79</v>
       </c>
@@ -1228,7 +3011,7 @@
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="5" t="s">
         <v>80</v>
       </c>
@@ -1261,7 +3044,7 @@
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="5" t="s">
         <v>81</v>
       </c>
@@ -1294,7 +3077,7 @@
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="5" t="s">
         <v>82</v>
       </c>
@@ -1327,7 +3110,7 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1362,7 +3145,7 @@
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="5" t="s">
         <v>84</v>
       </c>
@@ -1395,7 +3178,7 @@
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
         <v>85</v>
       </c>
@@ -1428,7 +3211,7 @@
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="5" t="s">
         <v>86</v>
       </c>
@@ -1461,7 +3244,7 @@
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1496,7 +3279,7 @@
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>88</v>
       </c>
@@ -1529,7 +3312,7 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="5" t="s">
         <v>89</v>
       </c>
@@ -1562,7 +3345,7 @@
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="5" t="s">
         <v>90</v>
       </c>
@@ -1595,7 +3378,7 @@
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>91</v>
       </c>
@@ -1628,7 +3411,7 @@
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>92</v>
       </c>
@@ -1661,7 +3444,7 @@
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="5" t="s">
         <v>93</v>
       </c>
@@ -1694,7 +3477,7 @@
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
         <v>94</v>
       </c>
@@ -1727,7 +3510,7 @@
       <c r="A19" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="5" t="s">
         <v>95</v>
       </c>
@@ -1760,7 +3543,7 @@
       <c r="A20" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +3576,7 @@
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
         <v>96</v>
       </c>
@@ -1826,7 +3609,7 @@
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="5" t="s">
         <v>97</v>
       </c>
@@ -1859,7 +3642,7 @@
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="5" t="s">
         <v>98</v>
       </c>
@@ -1892,7 +3675,7 @@
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="5" t="s">
         <v>99</v>
       </c>
@@ -1925,7 +3708,7 @@
       <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="5" t="s">
         <v>100</v>
       </c>
@@ -1958,7 +3741,7 @@
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="5" t="s">
         <v>101</v>
       </c>
@@ -1991,7 +3774,7 @@
       <c r="A27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="9" t="s">
         <v>75</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -2026,7 +3809,7 @@
       <c r="A28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="5" t="s">
         <v>93</v>
       </c>
@@ -2059,7 +3842,7 @@
       <c r="A29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="9"/>
       <c r="C29" s="5" t="s">
         <v>87</v>
       </c>
@@ -2092,7 +3875,7 @@
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="9"/>
       <c r="C30" s="5" t="s">
         <v>103</v>
       </c>
@@ -2125,7 +3908,7 @@
       <c r="A31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="5" t="s">
         <v>89</v>
       </c>
@@ -2158,7 +3941,7 @@
       <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="5" t="s">
         <v>88</v>
       </c>
@@ -2191,7 +3974,7 @@
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
@@ -2226,7 +4009,7 @@
       <c r="A34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="5" t="s">
         <v>105</v>
       </c>
@@ -2259,7 +4042,7 @@
       <c r="A35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="5" t="s">
         <v>106</v>
       </c>
@@ -2292,7 +4075,7 @@
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="5" t="s">
         <v>107</v>
       </c>
@@ -2325,7 +4108,7 @@
       <c r="A37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="6"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="5" t="s">
         <v>108</v>
       </c>
@@ -2358,7 +4141,7 @@
       <c r="A38" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="5" t="s">
         <v>109</v>
       </c>
@@ -2391,7 +4174,7 @@
       <c r="A39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="5" t="s">
         <v>110</v>
       </c>
@@ -2424,7 +4207,7 @@
       <c r="A40" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="6"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="5" t="s">
         <v>111</v>
       </c>
@@ -2457,7 +4240,7 @@
       <c r="A41" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="6"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="5" t="s">
         <v>112</v>
       </c>
@@ -2490,7 +4273,7 @@
       <c r="A42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="6"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="5" t="s">
         <v>113</v>
       </c>
@@ -2523,7 +4306,7 @@
       <c r="A43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C43" s="5" t="s">
@@ -2558,7 +4341,7 @@
       <c r="A44" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="5" t="s">
         <v>115</v>
       </c>
@@ -2591,7 +4374,7 @@
       <c r="A45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="5" t="s">
         <v>116</v>
       </c>
@@ -2624,7 +4407,7 @@
       <c r="A46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="5" t="s">
         <v>117</v>
       </c>
@@ -2657,7 +4440,7 @@
       <c r="A47" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="5" t="s">
         <v>118</v>
       </c>
@@ -2690,7 +4473,7 @@
       <c r="A48" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="5" t="s">
         <v>119</v>
       </c>
@@ -2723,7 +4506,7 @@
       <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="5" t="s">
         <v>120</v>
       </c>
@@ -2756,7 +4539,7 @@
       <c r="A50" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="5" t="s">
         <v>121</v>
       </c>
@@ -2789,7 +4572,7 @@
       <c r="A51" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="5" t="s">
         <v>122</v>
       </c>
@@ -2822,7 +4605,7 @@
       <c r="A52" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="5" t="s">
         <v>123</v>
       </c>
@@ -2855,7 +4638,7 @@
       <c r="A53" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="6"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="5" t="s">
         <v>124</v>
       </c>
@@ -2888,7 +4671,7 @@
       <c r="A54" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="6"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="5" t="s">
         <v>125</v>
       </c>
@@ -2921,7 +4704,7 @@
       <c r="A55" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="6"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="5" t="s">
         <v>126</v>
       </c>
@@ -2954,7 +4737,7 @@
       <c r="A56" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B56" s="6"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="5" t="s">
         <v>127</v>
       </c>
@@ -2987,7 +4770,7 @@
       <c r="A57" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="6"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="5" t="s">
         <v>128</v>
       </c>
@@ -3020,7 +4803,7 @@
       <c r="A58" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="5" t="s">
         <v>129</v>
       </c>
@@ -3053,7 +4836,7 @@
       <c r="A59" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="6"/>
+      <c r="B59" s="9"/>
       <c r="C59" s="5" t="s">
         <v>130</v>
       </c>
@@ -3086,7 +4869,7 @@
       <c r="A60" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="9"/>
       <c r="C60" s="5" t="s">
         <v>131</v>
       </c>
@@ -3119,7 +4902,7 @@
       <c r="A61" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="6"/>
+      <c r="B61" s="9"/>
       <c r="C61" s="5" t="s">
         <v>132</v>
       </c>
@@ -3152,7 +4935,7 @@
       <c r="A62" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="9"/>
       <c r="C62" s="5" t="s">
         <v>133</v>
       </c>
@@ -3183,14 +4966,2257 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B43:B62"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B26"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="B33:B42"/>
-    <mergeCell ref="B43:B62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F3" t="s">
+        <v>319</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>387</v>
+      </c>
+      <c r="E4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F4" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" t="s">
+        <v>318</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>389</v>
+      </c>
+      <c r="E6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" t="s">
+        <v>320</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>390</v>
+      </c>
+      <c r="E7" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" t="s">
+        <v>322</v>
+      </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E9" t="s">
+        <v>264</v>
+      </c>
+      <c r="F9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F10" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" t="s">
+        <v>325</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" t="s">
+        <v>326</v>
+      </c>
+      <c r="G12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13" t="s">
+        <v>322</v>
+      </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>253</v>
+      </c>
+      <c r="E14" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" t="s">
+        <v>327</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" t="s">
+        <v>270</v>
+      </c>
+      <c r="F15" t="s">
+        <v>322</v>
+      </c>
+      <c r="G15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" t="s">
+        <v>271</v>
+      </c>
+      <c r="F16" t="s">
+        <v>328</v>
+      </c>
+      <c r="G16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>256</v>
+      </c>
+      <c r="E17" t="s">
+        <v>272</v>
+      </c>
+      <c r="F17" t="s">
+        <v>329</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>273</v>
+      </c>
+      <c r="F18" t="s">
+        <v>330</v>
+      </c>
+      <c r="G18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" t="s">
+        <v>274</v>
+      </c>
+      <c r="F19" t="s">
+        <v>331</v>
+      </c>
+      <c r="G19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>275</v>
+      </c>
+      <c r="F20" t="s">
+        <v>332</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
+        <v>276</v>
+      </c>
+      <c r="F21" t="s">
+        <v>333</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>391</v>
+      </c>
+      <c r="E22" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>245</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>392</v>
+      </c>
+      <c r="E23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F23" t="s">
+        <v>335</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>245</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>393</v>
+      </c>
+      <c r="E24" t="s">
+        <v>279</v>
+      </c>
+      <c r="F24" t="s">
+        <v>336</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>245</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>394</v>
+      </c>
+      <c r="E25" t="s">
+        <v>280</v>
+      </c>
+      <c r="F25" t="s">
+        <v>337</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>395</v>
+      </c>
+      <c r="E26" t="s">
+        <v>281</v>
+      </c>
+      <c r="F26" t="s">
+        <v>338</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>245</v>
+      </c>
+      <c r="C27" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>396</v>
+      </c>
+      <c r="E27" t="s">
+        <v>282</v>
+      </c>
+      <c r="F27" t="s">
+        <v>339</v>
+      </c>
+      <c r="G27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>245</v>
+      </c>
+      <c r="C28" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F28" t="s">
+        <v>340</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>245</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>398</v>
+      </c>
+      <c r="E29" t="s">
+        <v>284</v>
+      </c>
+      <c r="F29" t="s">
+        <v>341</v>
+      </c>
+      <c r="G29" t="s">
+        <v>135</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>399</v>
+      </c>
+      <c r="E30" t="s">
+        <v>285</v>
+      </c>
+      <c r="F30" t="s">
+        <v>342</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>400</v>
+      </c>
+      <c r="E31" t="s">
+        <v>286</v>
+      </c>
+      <c r="F31" t="s">
+        <v>343</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>245</v>
+      </c>
+      <c r="C32" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>401</v>
+      </c>
+      <c r="E32" t="s">
+        <v>287</v>
+      </c>
+      <c r="F32" t="s">
+        <v>327</v>
+      </c>
+      <c r="G32" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>245</v>
+      </c>
+      <c r="C33" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>402</v>
+      </c>
+      <c r="E33" t="s">
+        <v>288</v>
+      </c>
+      <c r="F33" t="s">
+        <v>344</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>245</v>
+      </c>
+      <c r="C34" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>403</v>
+      </c>
+      <c r="E34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F34" t="s">
+        <v>345</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>404</v>
+      </c>
+      <c r="E35" t="s">
+        <v>290</v>
+      </c>
+      <c r="F35" t="s">
+        <v>346</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>245</v>
+      </c>
+      <c r="C36" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>405</v>
+      </c>
+      <c r="E36" t="s">
+        <v>291</v>
+      </c>
+      <c r="F36" t="s">
+        <v>327</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>406</v>
+      </c>
+      <c r="E37" t="s">
+        <v>292</v>
+      </c>
+      <c r="F37" t="s">
+        <v>347</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" t="s">
+        <v>293</v>
+      </c>
+      <c r="F38" t="s">
+        <v>348</v>
+      </c>
+      <c r="G38" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>246</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F39" t="s">
+        <v>349</v>
+      </c>
+      <c r="G39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" t="s">
+        <v>295</v>
+      </c>
+      <c r="F40" t="s">
+        <v>350</v>
+      </c>
+      <c r="G40" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>384</v>
+      </c>
+      <c r="E41" t="s">
+        <v>296</v>
+      </c>
+      <c r="F41" t="s">
+        <v>351</v>
+      </c>
+      <c r="G41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" t="s">
+        <v>297</v>
+      </c>
+      <c r="F42" t="s">
+        <v>352</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" t="s">
+        <v>298</v>
+      </c>
+      <c r="F43" t="s">
+        <v>353</v>
+      </c>
+      <c r="G43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" t="s">
+        <v>299</v>
+      </c>
+      <c r="F44" t="s">
+        <v>354</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" t="s">
+        <v>300</v>
+      </c>
+      <c r="F45" t="s">
+        <v>355</v>
+      </c>
+      <c r="G45" t="s">
+        <v>136</v>
+      </c>
+      <c r="H45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" t="s">
+        <v>301</v>
+      </c>
+      <c r="F46" t="s">
+        <v>356</v>
+      </c>
+      <c r="G46" t="s">
+        <v>137</v>
+      </c>
+      <c r="H46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" t="s">
+        <v>302</v>
+      </c>
+      <c r="F47" t="s">
+        <v>357</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s">
+        <v>303</v>
+      </c>
+      <c r="F48" t="s">
+        <v>358</v>
+      </c>
+      <c r="G48" t="s">
+        <v>138</v>
+      </c>
+      <c r="H48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" t="s">
+        <v>304</v>
+      </c>
+      <c r="F49" t="s">
+        <v>359</v>
+      </c>
+      <c r="G49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" t="s">
+        <v>305</v>
+      </c>
+      <c r="F50" t="s">
+        <v>360</v>
+      </c>
+      <c r="G50" t="s">
+        <v>139</v>
+      </c>
+      <c r="H50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" t="s">
+        <v>306</v>
+      </c>
+      <c r="F51" t="s">
+        <v>361</v>
+      </c>
+      <c r="G51" t="s">
+        <v>138</v>
+      </c>
+      <c r="H51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" t="s">
+        <v>307</v>
+      </c>
+      <c r="F52" t="s">
+        <v>362</v>
+      </c>
+      <c r="G52" t="s">
+        <v>138</v>
+      </c>
+      <c r="H52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" t="s">
+        <v>308</v>
+      </c>
+      <c r="F53" t="s">
+        <v>363</v>
+      </c>
+      <c r="G53" t="s">
+        <v>135</v>
+      </c>
+      <c r="H53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" t="s">
+        <v>309</v>
+      </c>
+      <c r="F54" t="s">
+        <v>364</v>
+      </c>
+      <c r="G54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="D55" t="s">
+        <v>126</v>
+      </c>
+      <c r="E55" t="s">
+        <v>310</v>
+      </c>
+      <c r="F55" t="s">
+        <v>365</v>
+      </c>
+      <c r="G55" t="s">
+        <v>136</v>
+      </c>
+      <c r="H55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D56" t="s">
+        <v>127</v>
+      </c>
+      <c r="E56" t="s">
+        <v>311</v>
+      </c>
+      <c r="F56" t="s">
+        <v>366</v>
+      </c>
+      <c r="G56" t="s">
+        <v>138</v>
+      </c>
+      <c r="H56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>128</v>
+      </c>
+      <c r="E57" t="s">
+        <v>312</v>
+      </c>
+      <c r="F57" t="s">
+        <v>367</v>
+      </c>
+      <c r="G57" t="s">
+        <v>136</v>
+      </c>
+      <c r="H57" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" t="s">
+        <v>313</v>
+      </c>
+      <c r="F58" t="s">
+        <v>368</v>
+      </c>
+      <c r="G58" t="s">
+        <v>138</v>
+      </c>
+      <c r="H58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>130</v>
+      </c>
+      <c r="E59" t="s">
+        <v>314</v>
+      </c>
+      <c r="F59" t="s">
+        <v>369</v>
+      </c>
+      <c r="G59" t="s">
+        <v>140</v>
+      </c>
+      <c r="H59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>131</v>
+      </c>
+      <c r="E60" t="s">
+        <v>315</v>
+      </c>
+      <c r="F60" t="s">
+        <v>370</v>
+      </c>
+      <c r="G60" t="s">
+        <v>140</v>
+      </c>
+      <c r="H60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>77</v>
+      </c>
+      <c r="C61" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>132</v>
+      </c>
+      <c r="E61" t="s">
+        <v>316</v>
+      </c>
+      <c r="F61" t="s">
+        <v>371</v>
+      </c>
+      <c r="G61" t="s">
+        <v>138</v>
+      </c>
+      <c r="H61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" t="s">
+        <v>317</v>
+      </c>
+      <c r="F62" t="s">
+        <v>366</v>
+      </c>
+      <c r="G62" t="s">
+        <v>140</v>
+      </c>
+      <c r="H62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>373</v>
+      </c>
+      <c r="E3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F4" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>375</v>
+      </c>
+      <c r="E5" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>376</v>
+      </c>
+      <c r="E6" t="s">
+        <v>382</v>
+      </c>
+      <c r="F6" t="s">
+        <v>311</v>
+      </c>
+      <c r="G6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H6" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>377</v>
+      </c>
+      <c r="E7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G7" t="s">
+        <v>369</v>
+      </c>
+      <c r="H7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E8" t="s">
+        <v>382</v>
+      </c>
+      <c r="F8" t="s">
+        <v>308</v>
+      </c>
+      <c r="G8" t="s">
+        <v>363</v>
+      </c>
+      <c r="H8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" t="s">
+        <v>382</v>
+      </c>
+      <c r="F9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G9" t="s">
+        <v>368</v>
+      </c>
+      <c r="H9" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" t="s">
+        <v>382</v>
+      </c>
+      <c r="F10" t="s">
+        <v>315</v>
+      </c>
+      <c r="G10" t="s">
+        <v>370</v>
+      </c>
+      <c r="H10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>381</v>
+      </c>
+      <c r="E11" t="s">
+        <v>382</v>
+      </c>
+      <c r="F11" t="s">
+        <v>310</v>
+      </c>
+      <c r="G11" t="s">
+        <v>365</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>372</v>
+      </c>
+      <c r="E12" t="s">
+        <v>383</v>
+      </c>
+      <c r="F12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G12" t="s">
+        <v>354</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E13" t="s">
+        <v>383</v>
+      </c>
+      <c r="F13" t="s">
+        <v>300</v>
+      </c>
+      <c r="G13" t="s">
+        <v>355</v>
+      </c>
+      <c r="H13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>374</v>
+      </c>
+      <c r="E14" t="s">
+        <v>383</v>
+      </c>
+      <c r="F14" t="s">
+        <v>301</v>
+      </c>
+      <c r="G14" t="s">
+        <v>356</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>375</v>
+      </c>
+      <c r="E15" t="s">
+        <v>383</v>
+      </c>
+      <c r="F15" t="s">
+        <v>306</v>
+      </c>
+      <c r="G15" t="s">
+        <v>361</v>
+      </c>
+      <c r="H15" t="s">
+        <v>138</v>
+      </c>
+      <c r="I15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>376</v>
+      </c>
+      <c r="E16" t="s">
+        <v>383</v>
+      </c>
+      <c r="F16" t="s">
+        <v>307</v>
+      </c>
+      <c r="G16" t="s">
+        <v>362</v>
+      </c>
+      <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>377</v>
+      </c>
+      <c r="E17" t="s">
+        <v>383</v>
+      </c>
+      <c r="F17" t="s">
+        <v>304</v>
+      </c>
+      <c r="G17" t="s">
+        <v>359</v>
+      </c>
+      <c r="H17" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>378</v>
+      </c>
+      <c r="E18" t="s">
+        <v>383</v>
+      </c>
+      <c r="F18" t="s">
+        <v>302</v>
+      </c>
+      <c r="G18" t="s">
+        <v>357</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E19" t="s">
+        <v>383</v>
+      </c>
+      <c r="F19" t="s">
+        <v>303</v>
+      </c>
+      <c r="G19" t="s">
+        <v>358</v>
+      </c>
+      <c r="H19" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E20" t="s">
+        <v>383</v>
+      </c>
+      <c r="F20" t="s">
+        <v>305</v>
+      </c>
+      <c r="G20" t="s">
+        <v>360</v>
+      </c>
+      <c r="H20" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>381</v>
+      </c>
+      <c r="E21" t="s">
+        <v>383</v>
+      </c>
+      <c r="F21" t="s">
+        <v>298</v>
+      </c>
+      <c r="G21" t="s">
+        <v>353</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>